<commit_message>
final commit for Jayati's changes
</commit_message>
<xml_diff>
--- a/merged/fetaure_importance.xlsx
+++ b/merged/fetaure_importance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joey/Desktop/Bootcamp_Project/transplant-survival/merged/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F4EE4180-85D3-B84D-AD78-2EBB87AF5022}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D3D34BF-90C6-7B49-9F29-BA86F5752857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="17260" xr2:uid="{DEBE2BEA-6D2C-114F-A17A-E637AC20C17D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="48">
   <si>
     <t>Feature importance for 1_Year_cleaned.csv</t>
   </si>
@@ -141,9 +141,6 @@
   </si>
   <si>
     <t>Congenital, Rare, Familial, and Metaboli</t>
-  </si>
-  <si>
-    <t>******************************************************************</t>
   </si>
   <si>
     <t>Feature importance for 3_Year_cleaned.csv</t>
@@ -565,8 +562,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A635A5A1-429C-7D4B-AA4B-164B72E833EF}">
   <dimension ref="A1:B229"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A212" workbookViewId="0">
+      <selection activeCell="A229" sqref="A229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -860,13 +857,11 @@
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A38" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A38" s="1"/>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="40" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -1134,7 +1129,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B74" s="4">
         <v>7.8581999999999999E-2</v>
@@ -1149,13 +1144,11 @@
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A76" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A76" s="1"/>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -1423,7 +1416,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B112" s="4">
         <v>0.118684</v>
@@ -1438,13 +1431,11 @@
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A114" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A114" s="1"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="116" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -1712,7 +1703,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B150" s="4">
         <v>0.12237099999999999</v>
@@ -1727,13 +1718,11 @@
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A152" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A152" s="1"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="154" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -1753,7 +1742,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B157" s="4">
         <v>0</v>
@@ -2017,20 +2006,18 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B190" s="4">
         <v>0.13788700000000001</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A191" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A191" s="1"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="193" spans="1:2" ht="18" x14ac:dyDescent="0.2">
@@ -2066,7 +2053,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B198" s="4">
         <v>0</v>
@@ -2242,7 +2229,7 @@
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B220" s="4">
         <v>5.398E-2</v>
@@ -2274,7 +2261,7 @@
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B224" s="4">
         <v>6.5680000000000002E-2</v>
@@ -2290,7 +2277,7 @@
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B226" s="4">
         <v>7.0209999999999995E-2</v>
@@ -2298,7 +2285,7 @@
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B227" s="4">
         <v>7.7060000000000003E-2</v>
@@ -2306,16 +2293,14 @@
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B228" s="4">
         <v>8.0451999999999996E-2</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A229" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="A229" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>